<commit_message>
pontos notáveis - incremento na tabela de ranking
</commit_message>
<xml_diff>
--- a/dados/csv/2023/analise_descritiva/dados/sint_resumo_por_genero_2023.xlsx
+++ b/dados/csv/2023/analise_descritiva/dados/sint_resumo_por_genero_2023.xlsx
@@ -498,10 +498,10 @@
         <v>29</v>
       </c>
       <c r="E2" s="1">
-        <v>0.03295880149812734</v>
+        <v>3.295880149812734</v>
       </c>
       <c r="F2" s="1">
-        <v>0.6590909090909091</v>
+        <v>65.90909090909091</v>
       </c>
       <c r="G2" s="2">
         <v>710060.7787271431</v>
@@ -533,10 +533,10 @@
         <v>83</v>
       </c>
       <c r="E3" s="1">
-        <v>0.08764044943820225</v>
+        <v>8.764044943820224</v>
       </c>
       <c r="F3" s="1">
-        <v>0.7094017094017094</v>
+        <v>70.94017094017094</v>
       </c>
       <c r="G3" s="2">
         <v>4257136.762729836</v>
@@ -568,10 +568,10 @@
         <v>140</v>
       </c>
       <c r="E4" s="1">
-        <v>0.1565543071161049</v>
+        <v>15.65543071161049</v>
       </c>
       <c r="F4" s="1">
-        <v>0.6698564593301436</v>
+        <v>66.98564593301435</v>
       </c>
       <c r="G4" s="2">
         <v>3881052.70273276</v>
@@ -603,10 +603,10 @@
         <v>576</v>
       </c>
       <c r="E5" s="1">
-        <v>0.7183520599250937</v>
+        <v>71.83520599250937</v>
       </c>
       <c r="F5" s="1">
-        <v>0.6006256517205423</v>
+        <v>60.06256517205423</v>
       </c>
       <c r="G5" s="2">
         <v>15212724.00148597</v>
@@ -638,10 +638,10 @@
         <v>2</v>
       </c>
       <c r="E6" s="1">
-        <v>0.004494382022471911</v>
+        <v>0.4494382022471911</v>
       </c>
       <c r="F6" s="1">
-        <v>0.3333333333333333</v>
+        <v>33.33333333333333</v>
       </c>
       <c r="G6" s="2">
         <v>2305.581647320182</v>
@@ -673,10 +673,10 @@
         <v>69</v>
       </c>
       <c r="E7" s="1">
-        <v>0.04904632152588556</v>
+        <v>4.904632152588556</v>
       </c>
       <c r="F7" s="1">
-        <v>0.9583333333333334</v>
+        <v>95.83333333333334</v>
       </c>
       <c r="G7" s="2">
         <v>1479515.330087252</v>
@@ -708,10 +708,10 @@
         <v>440</v>
       </c>
       <c r="E8" s="1">
-        <v>0.2997275204359673</v>
+        <v>29.97275204359673</v>
       </c>
       <c r="F8" s="1">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="G8" s="2">
         <v>9259515.000981268</v>
@@ -743,10 +743,10 @@
         <v>176</v>
       </c>
       <c r="E9" s="1">
-        <v>0.1239782016348774</v>
+        <v>12.39782016348774</v>
       </c>
       <c r="F9" s="1">
-        <v>0.967032967032967</v>
+        <v>96.7032967032967</v>
       </c>
       <c r="G9" s="2">
         <v>1145985.994178716</v>
@@ -778,10 +778,10 @@
         <v>691</v>
       </c>
       <c r="E10" s="1">
-        <v>0.5197547683923706</v>
+        <v>51.97547683923705</v>
       </c>
       <c r="F10" s="1">
-        <v>0.9056356487549148</v>
+        <v>90.56356487549148</v>
       </c>
       <c r="G10" s="2">
         <v>6465887.695217357</v>
@@ -813,10 +813,10 @@
         <v>7</v>
       </c>
       <c r="E11" s="1">
-        <v>0.007493188010899182</v>
+        <v>0.7493188010899182</v>
       </c>
       <c r="F11" s="1">
-        <v>0.6363636363636364</v>
+        <v>63.63636363636363</v>
       </c>
       <c r="G11" s="2">
         <v>11227.91709450537</v>
@@ -848,10 +848,10 @@
         <v>7</v>
       </c>
       <c r="E12" s="1">
-        <v>0.04093567251461988</v>
+        <v>4.093567251461988</v>
       </c>
       <c r="F12" s="1">
-        <v>0.25</v>
+        <v>25</v>
       </c>
       <c r="G12" s="2">
         <v>1146.907757768185</v>
@@ -883,10 +883,10 @@
         <v>2</v>
       </c>
       <c r="E13" s="1">
-        <v>0.0131578947368421</v>
+        <v>1.31578947368421</v>
       </c>
       <c r="F13" s="1">
-        <v>0.2222222222222222</v>
+        <v>22.22222222222222</v>
       </c>
       <c r="G13" s="2">
         <v>1022.282285906739</v>
@@ -918,10 +918,10 @@
         <v>18</v>
       </c>
       <c r="E14" s="1">
-        <v>0.1008771929824561</v>
+        <v>10.08771929824561</v>
       </c>
       <c r="F14" s="1">
-        <v>0.2608695652173913</v>
+        <v>26.08695652173913</v>
       </c>
       <c r="G14" s="2">
         <v>5551.368744100646</v>
@@ -953,10 +953,10 @@
         <v>25</v>
       </c>
       <c r="E15" s="1">
-        <v>0.1476608187134503</v>
+        <v>14.76608187134503</v>
       </c>
       <c r="F15" s="1">
-        <v>0.2475247524752475</v>
+        <v>24.75247524752475</v>
       </c>
       <c r="G15" s="2">
         <v>9304.802663330058</v>
@@ -988,10 +988,10 @@
         <v>100</v>
       </c>
       <c r="E16" s="1">
-        <v>0.6973684210526315</v>
+        <v>69.73684210526315</v>
       </c>
       <c r="F16" s="1">
-        <v>0.209643605870021</v>
+        <v>20.96436058700209</v>
       </c>
       <c r="G16" s="2">
         <v>26161.59630367918</v>

</xml_diff>